<commit_message>
Update code and data for macro controls
</commit_message>
<xml_diff>
--- a/OfficeMacroControl/CodeGen/Mitigations-All-Unedited.xlsx
+++ b/OfficeMacroControl/CodeGen/Mitigations-All-Unedited.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F140C21B-61B6-4F83-B4ED-F1B5B18AE103}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\AaronLockerWork\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{E3F750C3-DC10-4839-BE96-AA153D1900BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{C9C958A1-5228-4DFD-B0CF-114EF6E0C8CE}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{450D5A40-8661-4F67-BFC8-80334B9645C2}"/>
   </bookViews>
   <sheets>
     <sheet name="Policy Analyzer" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Policy Analyzer'!$A$1:$AS$81</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Policy Analyzer'!$A$1:$AS$83</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,6 +30,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3645" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3735" uniqueCount="196">
   <si>
     <t>Policy Config</t>
   </si>
@@ -201,7 +208,7 @@
     <t>Microsoft Access 2016\Application Settings\Security\Trust Center\</t>
   </si>
   <si>
-    <t>Block macros from running in Office files from the Internet</t>
+    <t>Block macros from running in Office files from the internet</t>
   </si>
   <si>
     <t>HKCU</t>
@@ -426,24 +433,24 @@
     <t>software\policies\microsoft\office\16.0\excel\security\trusted locations</t>
   </si>
   <si>
+    <t>Microsoft Project 2016\Project Options\Security\Trust Center\</t>
+  </si>
+  <si>
+    <t>software\policies\microsoft\office\16.0\ms project\security</t>
+  </si>
+  <si>
     <t>Microsoft Project 2016\Project Options\Security\</t>
   </si>
   <si>
     <t>Previous-version file formats</t>
   </si>
   <si>
-    <t>software\policies\microsoft\office\16.0\ms project\security</t>
-  </si>
-  <si>
     <t>legacyfiles</t>
   </si>
   <si>
     <t>Do not open or save</t>
   </si>
   <si>
-    <t>Microsoft Project 2016\Project Options\Security\Trust Center\</t>
-  </si>
-  <si>
     <t>software\policies\microsoft\office\16.0\ms project\security\trusted locations</t>
   </si>
   <si>
@@ -612,138 +619,40 @@
     <t>vbaoff</t>
   </si>
   <si>
-    <t>Windows Components\Microsoft Defender Antivirus\Real-time Protection\</t>
-  </si>
-  <si>
-    <t>Turn off real-time protection</t>
-  </si>
-  <si>
     <t>Software\Policies\Microsoft\Windows Defender\Real-Time Protection</t>
   </si>
   <si>
     <t>DisableRealtimeMonitoring</t>
   </si>
   <si>
-    <t>Disabled</t>
-  </si>
-  <si>
-    <t>Windows Components\Microsoft Defender Antivirus\Microsoft Defender Exploit Guard\Attack Surface Reduction\</t>
-  </si>
-  <si>
-    <t>Configure Attack Surface Reduction rules</t>
-  </si>
-  <si>
     <t>Software\Policies\Microsoft\Windows Defender\Windows Defender Exploit Guard\ASR</t>
   </si>
   <si>
     <t>ExploitGuard_ASR_Rules</t>
   </si>
   <si>
-    <t>Configure Attack Surface Reduction rules --&gt; Set the state for each ASR rule:</t>
-  </si>
-  <si>
     <t>Software\Policies\Microsoft\Windows Defender\Windows Defender Exploit Guard\ASR\Rules</t>
   </si>
   <si>
     <t>26190899-1602-49e8-8b27-eb1d0a1ce869</t>
   </si>
   <si>
-    <t>Rule: Block Office communication application from creating child processes_x000D_
-State: Audit</t>
-  </si>
-  <si>
     <t>REG_SZ</t>
   </si>
   <si>
-    <t>Rule: Block Office communication application from creating child processes_x000D_
-State: Block (enable ASR rule)</t>
-  </si>
-  <si>
-    <t>Rule: Block Office communication application from creating child processes_x000D_
-State: Disable</t>
-  </si>
-  <si>
     <t>6</t>
   </si>
   <si>
-    <t>Rule: Block Office communication application from creating child processes_x000D_
-State: Unrecognized code (6)</t>
-  </si>
-  <si>
     <t>3b576869-a4ec-4529-8536-b80a7769e899</t>
   </si>
   <si>
-    <t>Rule: Block Office applications from creating executable content_x000D_
-State: Audit</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from creating executable content_x000D_
-State: Block (enable ASR rule)</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from creating executable content_x000D_
-State: Disable</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from creating executable content_x000D_
-State: Unrecognized code (6)</t>
-  </si>
-  <si>
     <t>75668c1f-73b5-4cf0-bb93-3ecf5cb7cc84</t>
   </si>
   <si>
-    <t>Rule: Block Office applications from injecting code into other processes_x000D_
-State: Audit</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from injecting code into other processes_x000D_
-State: Block (enable ASR rule)</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from injecting code into other processes_x000D_
-State: Disable</t>
-  </si>
-  <si>
-    <t>Rule: Block Office applications from injecting code into other processes_x000D_
-State: Unrecognized code (6)</t>
-  </si>
-  <si>
     <t>92E97FA1-2EDF-4476-BDD6-9DD0B4DDDC7B</t>
   </si>
   <si>
-    <t>Rule: Block Win32 API calls from Office macro_x000D_
-State: Audit</t>
-  </si>
-  <si>
-    <t>Rule: Block Win32 API calls from Office macro_x000D_
-State: Block (enable ASR rule)</t>
-  </si>
-  <si>
-    <t>Rule: Block Win32 API calls from Office macro_x000D_
-State: Disable</t>
-  </si>
-  <si>
-    <t>Rule: Block Win32 API calls from Office macro_x000D_
-State: Unrecognized code (6)</t>
-  </si>
-  <si>
     <t>d4f940ab-401b-4efc-aadc-ad5f3c50688a</t>
-  </si>
-  <si>
-    <t>Rule: Block all Office applications from creating child processes_x000D_
-State: Audit</t>
-  </si>
-  <si>
-    <t>Rule: Block all Office applications from creating child processes_x000D_
-State: Block (enable ASR rule)</t>
-  </si>
-  <si>
-    <t>Rule: Block all Office applications from creating child processes_x000D_
-State: Disable</t>
-  </si>
-  <si>
-    <t>Rule: Block all Office applications from creating child processes_x000D_
-State: Unrecognized code (6)</t>
   </si>
 </sst>
 </file>
@@ -754,7 +663,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -762,7 +671,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -814,7 +723,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -834,9 +743,6 @@
     <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -855,9 +761,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -865,39 +771,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="156082"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="E97132"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="196B24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -949,7 +855,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1001,7 +907,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1060,13 +966,6 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -1075,6 +974,13 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1139,71 +1045,91 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8F6764E-98B1-4B6F-BCAC-555F620D17CC}">
-  <dimension ref="A1:AS81"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D49BD7-D2A7-4293-9B97-33DD7FC4DF56}">
+  <dimension ref="A1:AS83"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="50.81640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="12.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="38.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="50.81640625" style="1" customWidth="1"/>
-    <col min="20" max="20" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="32.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="45.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="40.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="45.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="32.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="45.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="36.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="11.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="33.1796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="21.81640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="10.90625" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="23" style="1" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="33" style="1" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="28.453125" style="1" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="29.36328125" style="1" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="12.08984375" style="1" bestFit="1" customWidth="1"/>
-    <col min="46" max="16384" width="8.90625" style="1"/>
+    <col min="1" max="1" width="20.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="50.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="12.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.6328125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="38.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7265625" style="1"/>
+    <col min="9" max="9" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" style="1"/>
+    <col min="12" max="12" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="9.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.7265625" style="1"/>
+    <col min="18" max="18" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="50.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="31.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="42.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="39" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="42.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="30.90625" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="42.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="34.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="10.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="32.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="10.54296875" style="1" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="22.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="30.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="27.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="27.36328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="11.6328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="46" max="16384" width="8.7265625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" ht="87" x14ac:dyDescent="0.35">
@@ -1345,58 +1271,58 @@
     </row>
     <row r="2" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>179</v>
+        <v>51</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>180</v>
+        <v>51</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>51</v>
+        <v>185</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="I2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>57</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="S2" s="5" t="s">
         <v>51</v>
@@ -1452,14 +1378,14 @@
       <c r="AJ2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AK2" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>53</v>
+      <c r="AK2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AM2" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AN2" s="5" t="s">
         <v>51</v>
@@ -1482,28 +1408,28 @@
     </row>
     <row r="3" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>190</v>
+        <v>51</v>
       </c>
       <c r="D3" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>52</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I3" s="4" t="s">
         <v>54</v>
@@ -1512,7 +1438,7 @@
         <v>52</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="L3" s="4" t="s">
         <v>54</v>
@@ -1521,7 +1447,7 @@
         <v>52</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="O3" s="4" t="s">
         <v>54</v>
@@ -1530,7 +1456,7 @@
         <v>52</v>
       </c>
       <c r="Q3" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="R3" s="4" t="s">
         <v>54</v>
@@ -1617,60 +1543,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:45" ht="203" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D4" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="G4" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H4" s="7" t="s">
-        <v>196</v>
+      <c r="H4" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J4" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K4" s="7" t="s">
-        <v>198</v>
+      <c r="K4" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M4" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="7" t="s">
-        <v>199</v>
+      <c r="N4" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="O4" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="P4" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q4" s="7" t="s">
-        <v>201</v>
+        <v>191</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="R4" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S4" s="5" t="s">
         <v>51</v>
@@ -1754,60 +1680,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:45" ht="174" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D5" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F5" s="4" t="s">
-        <v>202</v>
+        <v>192</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H5" s="7" t="s">
-        <v>203</v>
+      <c r="H5" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K5" s="7" t="s">
-        <v>204</v>
+      <c r="K5" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N5" s="7" t="s">
-        <v>205</v>
+      <c r="N5" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="O5" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="P5" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q5" s="7" t="s">
-        <v>206</v>
+        <v>191</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="R5" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S5" s="5" t="s">
         <v>51</v>
@@ -1891,60 +1817,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:45" ht="188.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D6" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G6" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H6" s="7" t="s">
-        <v>208</v>
+      <c r="H6" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I6" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J6" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="7" t="s">
-        <v>209</v>
+      <c r="K6" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M6" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N6" s="7" t="s">
-        <v>210</v>
+      <c r="N6" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="O6" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="P6" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q6" s="7" t="s">
-        <v>211</v>
+        <v>191</v>
+      </c>
+      <c r="Q6" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="R6" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S6" s="5" t="s">
         <v>51</v>
@@ -2028,60 +1954,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:45" ht="145" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A7" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D7" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E7" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>194</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>212</v>
       </c>
       <c r="G7" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H7" s="7" t="s">
-        <v>213</v>
+      <c r="H7" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I7" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="7" t="s">
-        <v>214</v>
+      <c r="K7" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M7" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N7" s="7" t="s">
-        <v>215</v>
+      <c r="N7" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="P7" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q7" s="7" t="s">
-        <v>216</v>
+        <v>191</v>
+      </c>
+      <c r="Q7" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="R7" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S7" s="5" t="s">
         <v>51</v>
@@ -2165,60 +2091,60 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:45" ht="174" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>178</v>
+        <v>51</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>189</v>
+        <v>51</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>193</v>
+        <v>51</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>217</v>
+        <v>195</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="H8" s="7" t="s">
-        <v>218</v>
+      <c r="H8" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="J8" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="K8" s="7" t="s">
-        <v>219</v>
+      <c r="K8" s="6" t="s">
+        <v>52</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="M8" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="N8" s="7" t="s">
-        <v>220</v>
+      <c r="N8" s="6" t="s">
+        <v>57</v>
       </c>
       <c r="O8" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="P8" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="Q8" s="7" t="s">
-        <v>221</v>
+        <v>191</v>
+      </c>
+      <c r="Q8" s="6" t="s">
+        <v>191</v>
       </c>
       <c r="R8" s="4" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="S8" s="5" t="s">
         <v>51</v>
@@ -2307,55 +2233,55 @@
         <v>178</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="D9" s="4" t="s">
         <v>181</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>188</v>
+        <v>183</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="J9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="K9" s="4" t="s">
-        <v>188</v>
+        <v>51</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="M9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="N9" s="4" t="s">
-        <v>188</v>
+        <v>51</v>
+      </c>
+      <c r="M9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>188</v>
+        <v>51</v>
+      </c>
+      <c r="P9" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q9" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="R9" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="S9" s="5" t="s">
         <v>51</v>
@@ -2411,14 +2337,14 @@
       <c r="AJ9" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AK9" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL9" s="5" t="s">
-        <v>51</v>
+      <c r="AK9" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL9" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="AM9" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AN9" s="5" t="s">
         <v>51</v>
@@ -7924,19 +7850,19 @@
         <v>45</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F50" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>51</v>
@@ -8041,7 +7967,7 @@
         <v>57</v>
       </c>
       <c r="AO50" s="4" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="AP50" s="4" t="s">
         <v>54</v>
@@ -8061,19 +7987,19 @@
         <v>45</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>69</v>
+        <v>47</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F51" s="4" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>51</v>
@@ -8111,14 +8037,14 @@
       <c r="R51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S51" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T51" s="5" t="s">
-        <v>51</v>
+      <c r="S51" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T51" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="U51" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="V51" s="5" t="s">
         <v>51</v>
@@ -8156,14 +8082,14 @@
       <c r="AG51" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AH51" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI51" s="4" t="s">
-        <v>53</v>
+      <c r="AH51" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI51" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AJ51" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AK51" s="5" t="s">
         <v>51</v>
@@ -8198,19 +8124,19 @@
         <v>45</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>124</v>
+        <v>128</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>51</v>
@@ -8257,32 +8183,32 @@
       <c r="U52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W52" s="4" t="s">
-        <v>67</v>
+      <c r="V52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W52" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="X52" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z52" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="Y52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z52" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AA52" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB52" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC52" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="AB52" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC52" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AD52" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE52" s="5" t="s">
         <v>51</v>
@@ -8293,14 +8219,14 @@
       <c r="AG52" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AH52" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI52" s="5" t="s">
-        <v>51</v>
+      <c r="AH52" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="AI52" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="AJ52" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AK52" s="5" t="s">
         <v>51</v>
@@ -8335,7 +8261,7 @@
         <v>45</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
       <c r="C53" s="4" t="s">
         <v>64</v>
@@ -8344,7 +8270,7 @@
         <v>48</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
       <c r="F53" s="4" t="s">
         <v>65</v>
@@ -8475,7 +8401,7 @@
         <v>140</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="D54" s="4" t="s">
         <v>48</v>
@@ -8484,7 +8410,7 @@
         <v>141</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="G54" s="5" t="s">
         <v>51</v>
@@ -8522,41 +8448,41 @@
       <c r="R54" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S54" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T54" s="5" t="s">
-        <v>51</v>
+      <c r="S54" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T54" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="U54" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V54" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W54" s="6" t="s">
-        <v>58</v>
+        <v>54</v>
+      </c>
+      <c r="V54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W54" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="X54" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y54" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z54" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="Y54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z54" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AA54" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB54" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC54" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
+      </c>
+      <c r="AB54" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC54" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AD54" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE54" s="5" t="s">
         <v>51</v>
@@ -8612,7 +8538,7 @@
         <v>140</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D55" s="4" t="s">
         <v>48</v>
@@ -8621,7 +8547,7 @@
         <v>141</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G55" s="5" t="s">
         <v>51</v>
@@ -8668,29 +8594,29 @@
       <c r="U55" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W55" s="6" t="s">
-        <v>58</v>
+      <c r="V55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W55" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="X55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y55" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z55" s="6" t="s">
-        <v>58</v>
+      <c r="Y55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z55" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AA55" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AB55" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC55" s="6" t="s">
-        <v>59</v>
+      <c r="AB55" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC55" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AD55" s="4" t="s">
         <v>54</v>
@@ -8749,7 +8675,7 @@
         <v>140</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>48</v>
@@ -8758,7 +8684,7 @@
         <v>141</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G56" s="5" t="s">
         <v>51</v>
@@ -8815,10 +8741,10 @@
         <v>54</v>
       </c>
       <c r="Y56" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Z56" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA56" s="4" t="s">
         <v>54</v>
@@ -8883,19 +8809,19 @@
         <v>45</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>47</v>
+        <v>60</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="G57" s="5" t="s">
         <v>51</v>
@@ -8933,41 +8859,41 @@
       <c r="R57" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S57" s="4" t="s">
+      <c r="S57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T57" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U57" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V57" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W57" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="X57" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="Y57" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z57" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA57" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB57" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="T57" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="U57" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="V57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="X57" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA57" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB57" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC57" s="5" t="s">
-        <v>51</v>
+      <c r="AC57" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD57" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE57" s="5" t="s">
         <v>51</v>
@@ -9020,19 +8946,19 @@
         <v>45</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>153</v>
+        <v>141</v>
       </c>
       <c r="F58" s="4" t="s">
-        <v>71</v>
+        <v>56</v>
       </c>
       <c r="G58" s="5" t="s">
         <v>51</v>
@@ -9079,32 +9005,32 @@
       <c r="U58" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V58" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W58" s="5" t="s">
-        <v>51</v>
+      <c r="V58" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W58" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="X58" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y58" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z58" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Y58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z58" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AA58" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB58" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC58" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="AB58" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC58" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD58" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE58" s="5" t="s">
         <v>51</v>
@@ -9115,14 +9041,14 @@
       <c r="AG58" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AH58" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="AI58" s="4" t="s">
-        <v>53</v>
+      <c r="AH58" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI58" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AJ58" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AK58" s="5" t="s">
         <v>51</v>
@@ -9160,7 +9086,7 @@
         <v>142</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D59" s="4" t="s">
         <v>48</v>
@@ -9169,7 +9095,7 @@
         <v>143</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G59" s="5" t="s">
         <v>51</v>
@@ -9207,41 +9133,41 @@
       <c r="R59" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S59" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T59" s="5" t="s">
-        <v>51</v>
+      <c r="S59" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T59" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="U59" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V59" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W59" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="V59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W59" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="X59" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y59" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z59" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="Y59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z59" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AA59" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB59" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC59" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="AB59" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC59" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AD59" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE59" s="5" t="s">
         <v>51</v>
@@ -9297,16 +9223,16 @@
         <v>142</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>62</v>
+        <v>69</v>
       </c>
       <c r="D60" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>143</v>
+        <v>153</v>
       </c>
       <c r="F60" s="4" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="G60" s="5" t="s">
         <v>51</v>
@@ -9353,50 +9279,50 @@
       <c r="U60" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V60" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W60" s="6" t="s">
-        <v>58</v>
+      <c r="V60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W60" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="X60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y60" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z60" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
+      </c>
+      <c r="Y60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z60" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AA60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB60" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD60" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF60" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG60" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH60" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AC60" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD60" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE60" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF60" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG60" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH60" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI60" s="5" t="s">
-        <v>51</v>
+      <c r="AI60" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="AJ60" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AK60" s="5" t="s">
         <v>51</v>
@@ -9434,7 +9360,7 @@
         <v>142</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>48</v>
@@ -9443,7 +9369,7 @@
         <v>143</v>
       </c>
       <c r="F61" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G61" s="5" t="s">
         <v>51</v>
@@ -9490,29 +9416,29 @@
       <c r="U61" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V61" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W61" s="6" t="s">
-        <v>58</v>
+      <c r="V61" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W61" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="X61" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y61" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z61" s="6" t="s">
-        <v>58</v>
+      <c r="Y61" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z61" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AA61" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AB61" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC61" s="6" t="s">
-        <v>59</v>
+      <c r="AB61" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC61" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AD61" s="4" t="s">
         <v>54</v>
@@ -9571,7 +9497,7 @@
         <v>142</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D62" s="4" t="s">
         <v>48</v>
@@ -9580,7 +9506,7 @@
         <v>143</v>
       </c>
       <c r="F62" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G62" s="5" t="s">
         <v>51</v>
@@ -9637,10 +9563,10 @@
         <v>54</v>
       </c>
       <c r="Y62" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Z62" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA62" s="4" t="s">
         <v>54</v>
@@ -9705,19 +9631,19 @@
         <v>45</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>145</v>
+        <v>60</v>
       </c>
       <c r="D63" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F63" s="4" t="s">
-        <v>147</v>
+        <v>61</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>51</v>
@@ -9764,32 +9690,32 @@
       <c r="U63" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V63" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W63" s="5" t="s">
-        <v>51</v>
+      <c r="V63" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W63" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="X63" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y63" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z63" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Y63" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z63" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="AA63" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB63" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC63" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="AB63" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC63" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD63" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE63" s="5" t="s">
         <v>51</v>
@@ -9818,14 +9744,14 @@
       <c r="AM63" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN63" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO63" s="4" t="s">
-        <v>148</v>
+      <c r="AN63" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO63" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AP63" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ63" s="5" t="s">
         <v>51</v>
@@ -9842,19 +9768,19 @@
         <v>45</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>149</v>
+        <v>55</v>
       </c>
       <c r="D64" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>150</v>
+        <v>56</v>
       </c>
       <c r="G64" s="5" t="s">
         <v>51</v>
@@ -9901,32 +9827,32 @@
       <c r="U64" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V64" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W64" s="5" t="s">
-        <v>51</v>
+      <c r="V64" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W64" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="X64" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y64" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z64" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Y64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z64" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AA64" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB64" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC64" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="AB64" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC64" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD64" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE64" s="5" t="s">
         <v>51</v>
@@ -9955,14 +9881,14 @@
       <c r="AM64" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN64" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO64" s="4" t="s">
-        <v>148</v>
+      <c r="AN64" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO64" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AP64" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ64" s="5" t="s">
         <v>51</v>
@@ -9982,7 +9908,7 @@
         <v>144</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>48</v>
@@ -9991,7 +9917,7 @@
         <v>146</v>
       </c>
       <c r="F65" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G65" s="5" t="s">
         <v>51</v>
@@ -10116,19 +10042,19 @@
         <v>45</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>47</v>
+        <v>149</v>
       </c>
       <c r="D66" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F66" s="4" t="s">
-        <v>50</v>
+        <v>150</v>
       </c>
       <c r="G66" s="5" t="s">
         <v>51</v>
@@ -10166,14 +10092,14 @@
       <c r="R66" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S66" s="4" t="s">
-        <v>52</v>
-      </c>
-      <c r="T66" s="4" t="s">
-        <v>53</v>
+      <c r="S66" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T66" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="U66" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="V66" s="5" t="s">
         <v>51</v>
@@ -10229,14 +10155,14 @@
       <c r="AM66" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN66" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO66" s="5" t="s">
-        <v>51</v>
+      <c r="AN66" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO66" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="AP66" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AQ66" s="5" t="s">
         <v>51</v>
@@ -10253,19 +10179,19 @@
         <v>45</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D67" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="F67" s="4" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="G67" s="5" t="s">
         <v>51</v>
@@ -10366,23 +10292,23 @@
       <c r="AM67" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN67" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO67" s="5" t="s">
-        <v>51</v>
+      <c r="AN67" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO67" s="4" t="s">
+        <v>148</v>
       </c>
       <c r="AP67" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ67" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AR67" s="4" t="s">
-        <v>77</v>
+        <v>54</v>
+      </c>
+      <c r="AQ67" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR67" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AS67" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
     <row r="68" spans="1:45" x14ac:dyDescent="0.35">
@@ -10393,7 +10319,7 @@
         <v>154</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="D68" s="4" t="s">
         <v>48</v>
@@ -10402,7 +10328,7 @@
         <v>155</v>
       </c>
       <c r="F68" s="4" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="G68" s="5" t="s">
         <v>51</v>
@@ -10440,41 +10366,41 @@
       <c r="R68" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="S68" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T68" s="5" t="s">
-        <v>51</v>
+      <c r="S68" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="T68" s="4" t="s">
+        <v>53</v>
       </c>
       <c r="U68" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V68" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="W68" s="4" t="s">
-        <v>67</v>
+        <v>54</v>
+      </c>
+      <c r="V68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W68" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="X68" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y68" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z68" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="Y68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z68" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AA68" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB68" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="AC68" s="4" t="s">
-        <v>67</v>
+        <v>51</v>
+      </c>
+      <c r="AB68" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC68" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AD68" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AE68" s="5" t="s">
         <v>51</v>
@@ -10530,7 +10456,7 @@
         <v>154</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>62</v>
+        <v>156</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>48</v>
@@ -10539,7 +10465,7 @@
         <v>155</v>
       </c>
       <c r="F69" s="4" t="s">
-        <v>63</v>
+        <v>157</v>
       </c>
       <c r="G69" s="5" t="s">
         <v>51</v>
@@ -10586,77 +10512,77 @@
       <c r="U69" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V69" s="6" t="s">
+      <c r="V69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO69" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP69" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ69" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="W69" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="X69" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="Y69" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z69" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="AA69" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB69" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC69" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AD69" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG69" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AI69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AJ69" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AK69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM69" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP69" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ69" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR69" s="5" t="s">
-        <v>51</v>
+      <c r="AR69" s="4" t="s">
+        <v>77</v>
       </c>
       <c r="AS69" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:45" x14ac:dyDescent="0.35">
@@ -10667,7 +10593,7 @@
         <v>154</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>48</v>
@@ -10676,7 +10602,7 @@
         <v>155</v>
       </c>
       <c r="F70" s="4" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="G70" s="5" t="s">
         <v>51</v>
@@ -10723,29 +10649,29 @@
       <c r="U70" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V70" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="W70" s="6" t="s">
-        <v>58</v>
+      <c r="V70" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="W70" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="X70" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="Y70" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="Z70" s="6" t="s">
-        <v>58</v>
+      <c r="Y70" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z70" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AA70" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="AB70" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="AC70" s="6" t="s">
-        <v>59</v>
+      <c r="AB70" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC70" s="4" t="s">
+        <v>67</v>
       </c>
       <c r="AD70" s="4" t="s">
         <v>54</v>
@@ -10804,7 +10730,7 @@
         <v>154</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>55</v>
+        <v>62</v>
       </c>
       <c r="D71" s="4" t="s">
         <v>48</v>
@@ -10813,7 +10739,7 @@
         <v>155</v>
       </c>
       <c r="F71" s="4" t="s">
-        <v>56</v>
+        <v>63</v>
       </c>
       <c r="G71" s="5" t="s">
         <v>51</v>
@@ -10870,10 +10796,10 @@
         <v>54</v>
       </c>
       <c r="Y71" s="6" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="Z71" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="AA71" s="4" t="s">
         <v>54</v>
@@ -10938,19 +10864,19 @@
         <v>45</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>97</v>
+        <v>60</v>
       </c>
       <c r="D72" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F72" s="4" t="s">
-        <v>98</v>
+        <v>61</v>
       </c>
       <c r="G72" s="5" t="s">
         <v>51</v>
@@ -10997,32 +10923,32 @@
       <c r="U72" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V72" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W72" s="5" t="s">
-        <v>51</v>
+      <c r="V72" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W72" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="X72" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y72" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z72" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Y72" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z72" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="AA72" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB72" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC72" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="AB72" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC72" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD72" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE72" s="5" t="s">
         <v>51</v>
@@ -11051,14 +10977,14 @@
       <c r="AM72" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN72" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="AO72" s="4" t="s">
-        <v>99</v>
+      <c r="AN72" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO72" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AP72" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ72" s="5" t="s">
         <v>51</v>
@@ -11075,19 +11001,19 @@
         <v>45</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>166</v>
+        <v>55</v>
       </c>
       <c r="D73" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="F73" s="4" t="s">
-        <v>167</v>
+        <v>56</v>
       </c>
       <c r="G73" s="5" t="s">
         <v>51</v>
@@ -11134,32 +11060,32 @@
       <c r="U73" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="V73" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W73" s="5" t="s">
-        <v>51</v>
+      <c r="V73" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="W73" s="6" t="s">
+        <v>58</v>
       </c>
       <c r="X73" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y73" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z73" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="Y73" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z73" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AA73" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB73" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC73" s="5" t="s">
-        <v>51</v>
+        <v>54</v>
+      </c>
+      <c r="AB73" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC73" s="6" t="s">
+        <v>59</v>
       </c>
       <c r="AD73" s="4" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AE73" s="5" t="s">
         <v>51</v>
@@ -11188,14 +11114,14 @@
       <c r="AM73" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AN73" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="AO73" s="4" t="s">
-        <v>92</v>
+      <c r="AN73" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO73" s="5" t="s">
+        <v>51</v>
       </c>
       <c r="AP73" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="AQ73" s="5" t="s">
         <v>51</v>
@@ -11215,7 +11141,7 @@
         <v>158</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>160</v>
+        <v>97</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>48</v>
@@ -11224,7 +11150,7 @@
         <v>159</v>
       </c>
       <c r="F74" s="4" t="s">
-        <v>161</v>
+        <v>98</v>
       </c>
       <c r="G74" s="5" t="s">
         <v>51</v>
@@ -11326,10 +11252,10 @@
         <v>51</v>
       </c>
       <c r="AN74" s="4" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
       <c r="AO74" s="4" t="s">
-        <v>92</v>
+        <v>99</v>
       </c>
       <c r="AP74" s="4" t="s">
         <v>54</v>
@@ -11352,7 +11278,7 @@
         <v>158</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>162</v>
+        <v>166</v>
       </c>
       <c r="D75" s="4" t="s">
         <v>48</v>
@@ -11361,7 +11287,7 @@
         <v>159</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>163</v>
+        <v>167</v>
       </c>
       <c r="G75" s="5" t="s">
         <v>51</v>
@@ -11489,7 +11415,7 @@
         <v>158</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="D76" s="4" t="s">
         <v>48</v>
@@ -11498,7 +11424,7 @@
         <v>159</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="G76" s="5" t="s">
         <v>51</v>
@@ -11626,7 +11552,7 @@
         <v>158</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="D77" s="4" t="s">
         <v>48</v>
@@ -11635,7 +11561,7 @@
         <v>159</v>
       </c>
       <c r="F77" s="4" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G77" s="5" t="s">
         <v>51</v>
@@ -11763,7 +11689,7 @@
         <v>158</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D78" s="4" t="s">
         <v>48</v>
@@ -11772,7 +11698,7 @@
         <v>159</v>
       </c>
       <c r="F78" s="4" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G78" s="5" t="s">
         <v>51</v>
@@ -11900,7 +11826,7 @@
         <v>158</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D79" s="4" t="s">
         <v>48</v>
@@ -11909,7 +11835,7 @@
         <v>159</v>
       </c>
       <c r="F79" s="4" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="G79" s="5" t="s">
         <v>51</v>
@@ -12037,7 +11963,7 @@
         <v>158</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="D80" s="4" t="s">
         <v>48</v>
@@ -12046,7 +11972,7 @@
         <v>159</v>
       </c>
       <c r="F80" s="4" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="G80" s="5" t="s">
         <v>51</v>
@@ -12171,141 +12097,415 @@
         <v>45</v>
       </c>
       <c r="B81" s="4" t="s">
-        <v>176</v>
+        <v>158</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>69</v>
+        <v>172</v>
       </c>
       <c r="D81" s="4" t="s">
         <v>48</v>
       </c>
       <c r="E81" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F81" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="G81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM81" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN81" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO81" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP81" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR81" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS81" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="82" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A82" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C82" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="D82" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E82" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="F82" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AI82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AK82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM82" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN82" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AO82" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AP82" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AQ82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR82" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS82" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="83" spans="1:45" x14ac:dyDescent="0.35">
+      <c r="A83" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E83" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="F81" s="4" t="s">
+      <c r="F83" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="G81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="H81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="I81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="J81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="K81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="L81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="M81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="N81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="O81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="P81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="R81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="S81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="T81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="U81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="V81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="W81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="X81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Z81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AA81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AB81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AE81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AF81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AG81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AH81" s="4" t="s">
+      <c r="G83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="H83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="I83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="J83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="L83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="M83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="N83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="O83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="P83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="R83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="T83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="U83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="V83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="W83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="X83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AA83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AB83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AC83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AE83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AF83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AG83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AH83" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="AI81" s="4" t="s">
+      <c r="AI83" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="AJ81" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AK81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AL81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AM81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AP81" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AQ81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AR81" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="AS81" s="4" t="s">
+      <c r="AJ83" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AK83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AL83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AM83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AN83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AO83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AP83" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="AQ83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AR83" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS83" s="4" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AS81" xr:uid="{1C89D9DD-D0EA-4A5D-89EB-5A8817FB00A9}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS81">
+  <autoFilter ref="A1:AS83" xr:uid="{34D49BD7-D2A7-4293-9B97-33DD7FC4DF56}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AS83">
       <sortCondition ref="A1:A1048576"/>
       <sortCondition ref="B1:B1048576"/>
       <sortCondition ref="C1:C1048576"/>
@@ -12315,6 +12515,5 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
</xml_diff>